<commit_message>
Tweaks and merging of some calculations
</commit_message>
<xml_diff>
--- a/WorkerCalc.xlsx
+++ b/WorkerCalc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Whitefang Greytail\Documents\Visual Studio 2019\Projects\WG_HouseholdCapacityModifier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Whitefang Greytail\Documents\Visual Studio 2019\Projects\CS2_RealisticPopulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D0C6AF-0DB8-49BC-8232-E648B5DF27D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D806FC-78AA-4F3D-9D44-8DFBEA4DD4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="C1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -469,7 +469,7 @@
       </c>
       <c r="H4">
         <f>(C4*extra)*(D4*extra)*E4*F4*G4</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
       </c>
       <c r="E5">
         <f>E4</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <f>F4</f>
@@ -493,7 +493,7 @@
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H12" si="0">(C5*extra)*(D5*extra)*E5*F5*G5</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E12" si="1">E5</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F12" si="2">F5</f>
@@ -517,7 +517,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>13.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
@@ -541,7 +541,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
@@ -589,7 +589,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
@@ -613,7 +613,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
@@ -637,7 +637,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
@@ -661,7 +661,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reducing level 5 office and overall density in light of game mechanics
</commit_message>
<xml_diff>
--- a/WorkerCalc.xlsx
+++ b/WorkerCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Whitefang Greytail\Documents\Visual Studio 2019\Projects\CS2_RealisticPopulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D806FC-78AA-4F3D-9D44-8DFBEA4DD4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E351FD42-36C6-40DF-B4DE-867C17BB7A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="C1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,18 +672,18 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F26" si="4">10*(MIN(FLOOR((C15+D15)/2,1),6)-1)</f>
-        <v>10</v>
+        <f>MIN(FLOOR((C15+D15)/2,1),5)-1</f>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0.5</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H23" si="5">(C15*extra)*(D15*extra)*E15*F15*G15</f>
-        <v>50</v>
+        <f t="shared" ref="H15:H23" si="4">(C15*extra)*(D15*extra)*E15*F15*G15</f>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
@@ -695,19 +695,19 @@
       </c>
       <c r="E16">
         <f>E15</f>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" ref="F16:F26" si="5">(MIN(FLOOR((C16+D16)/2,1),6)-1)</f>
+        <v>1</v>
       </c>
       <c r="G16">
         <f>G15</f>
         <v>0.5</v>
       </c>
       <c r="H16">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="4"/>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
@@ -719,19 +719,19 @@
       </c>
       <c r="E17">
         <f t="shared" ref="E17:E26" si="6">E16</f>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="G17">
         <f t="shared" ref="G17:G24" si="7">G16</f>
         <v>0.5</v>
       </c>
       <c r="H17">
-        <f t="shared" si="5"/>
-        <v>300</v>
+        <f t="shared" si="4"/>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
@@ -743,19 +743,19 @@
       </c>
       <c r="E18">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="G18">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="H18">
-        <f t="shared" si="5"/>
-        <v>562.5</v>
+        <f t="shared" si="4"/>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
@@ -767,19 +767,19 @@
       </c>
       <c r="E19">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="G19">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="H19">
-        <f t="shared" si="5"/>
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>576</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
@@ -791,19 +791,19 @@
       </c>
       <c r="E20">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="G20">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="H20">
-        <f t="shared" si="5"/>
-        <v>750</v>
+        <f t="shared" si="4"/>
+        <v>720</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
@@ -815,19 +815,19 @@
       </c>
       <c r="E21">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
-        <v>40</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="G21">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="H21">
-        <f t="shared" si="5"/>
-        <v>1250</v>
+        <f t="shared" si="4"/>
+        <v>1200</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
@@ -839,19 +839,19 @@
       </c>
       <c r="E22">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
-        <v>40</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="G22">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="H22">
-        <f t="shared" si="5"/>
-        <v>1500</v>
+        <f t="shared" si="4"/>
+        <v>1440</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
@@ -863,19 +863,19 @@
       </c>
       <c r="E23">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>24</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
-        <v>50</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="G23">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="H23">
-        <f t="shared" si="5"/>
-        <v>2250</v>
+        <f t="shared" si="4"/>
+        <v>2160</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
@@ -886,12 +886,11 @@
         <v>9</v>
       </c>
       <c r="E24">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="F24">
-        <f t="shared" si="4"/>
-        <v>50</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="G24">
         <f t="shared" si="7"/>
@@ -899,7 +898,7 @@
       </c>
       <c r="H24">
         <f t="shared" ref="H24" si="8">(C24*extra)*(D24*extra)*E24*F24*G24</f>
-        <v>4500</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
@@ -911,11 +910,11 @@
       </c>
       <c r="E25">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
-        <v>50</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="G25">
         <f>G24</f>
@@ -923,7 +922,7 @@
       </c>
       <c r="H25">
         <f t="shared" ref="H25" si="9">(C25*extra)*(D25*extra)*E25*F25*G25</f>
-        <v>5000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
@@ -935,11 +934,11 @@
       </c>
       <c r="E26">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="F26">
-        <f t="shared" si="4"/>
-        <v>50</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="G26">
         <f>G25</f>
@@ -947,7 +946,7 @@
       </c>
       <c r="H26">
         <f>(C26*extra)*(D26*extra)*E26*F26*G26</f>
-        <v>10500</v>
+        <v>8400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing with these numbers
</commit_message>
<xml_diff>
--- a/WorkerCalc.xlsx
+++ b/WorkerCalc.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Whitefang Greytail\Documents\Visual Studio 2019\Projects\CS2_RealisticPopulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61582F0C-2FA6-40AB-AE8F-32BD45125EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FB9559-C77A-425B-99AF-C9EED3624E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Office" sheetId="1" r:id="rId1"/>
+    <sheet name="Residential" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="extra">Sheet1!$G$1</definedName>
+    <definedName name="extra">Office!$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>w</t>
   </si>
@@ -59,7 +60,22 @@
     <t>workerCell</t>
   </si>
   <si>
-    <t>extra</t>
+    <t>homes</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>lvlMult</t>
+  </si>
+  <si>
+    <t>high density</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>buildings</t>
   </si>
 </sst>
 </file>
@@ -411,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3C188A-A917-4627-9F8C-CA03B9A0C4A5}">
-  <dimension ref="C1:H26"/>
+  <dimension ref="C3:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,15 +439,7 @@
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -451,7 +459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>2</v>
       </c>
@@ -459,7 +467,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -468,11 +476,11 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f>(C4*extra)*(D4*extra)*E4*F4*G4</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+        <f>(C4)*(D4)*E4*F4*G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -481,7 +489,7 @@
       </c>
       <c r="E5">
         <f>E4</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <f>F4</f>
@@ -492,11 +500,11 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H12" si="0">(C5*extra)*(D5*extra)*E5*F5*G5</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H5:H12" si="0">(C5)*(D5)*E5*F5*G5</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -505,7 +513,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E12" si="1">E5</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F12" si="2">F5</f>
@@ -517,10 +525,10 @@
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -529,7 +537,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
@@ -541,10 +549,10 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>4</v>
       </c>
@@ -553,7 +561,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
@@ -565,34 +573,34 @@
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>5</v>
       </c>
@@ -601,7 +609,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
@@ -613,10 +621,10 @@
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>6</v>
       </c>
@@ -625,7 +633,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
@@ -637,10 +645,10 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>6</v>
       </c>
@@ -649,7 +657,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
@@ -661,10 +669,24 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>12000</v>
+      </c>
+      <c r="K14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>2</v>
       </c>
@@ -672,281 +694,993 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F15">
-        <f>MIN(FLOOR((C15+D15)/2,1),5)-1</f>
-        <v>1</v>
+        <f>(MIN(FLOOR((C15+D15)/2,1),5))</f>
+        <v>2</v>
       </c>
       <c r="G15">
         <v>0.5</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H23" si="4">(C15*extra)*(D15*extra)*E15*F15*G15</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+        <f>(C15)*(D15)*E15*F15*G15</f>
+        <v>64</v>
+      </c>
+      <c r="J15">
+        <f>12000*(H15/(C15*D15))</f>
+        <v>192000</v>
+      </c>
+      <c r="K15">
+        <f>12000/(C15*D15)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <f>E15</f>
-        <v>22.5</v>
+        <f t="shared" ref="E16:E26" si="4">E15</f>
+        <v>16</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F26" si="5">(MIN(FLOOR((C16+D16)/2,1),6)-1)</f>
-        <v>1</v>
+        <f t="shared" ref="F16:F29" si="5">(MIN(FLOOR((C16+D16)/2,1),5))</f>
+        <v>3</v>
       </c>
       <c r="G16">
-        <f>G15</f>
+        <f t="shared" ref="G16:G29" si="6">G15</f>
         <v>0.5</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+        <f>(C16)*(D16)*E16*F16*G16</f>
+        <v>192</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J29" si="7">12000*(H16/(C16*D16))</f>
+        <v>288000</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16:K29" si="8">12000/(C16*D16)</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E26" si="6">E16</f>
-        <v>22.5</v>
+        <f t="shared" si="4"/>
+        <v>16</v>
       </c>
       <c r="F17">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G24" si="7">G16</f>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H17:H29" si="9">(C17)*(D17)*E17*F17*G17</f>
+        <v>96</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="7"/>
+        <v>192000</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="8"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="9"/>
+        <v>288</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="7"/>
+        <v>288000</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="8"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="9"/>
+        <v>480</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="7"/>
+        <v>384000</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="9"/>
+        <v>576</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="7"/>
+        <v>384000</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="8"/>
+        <v>666.66666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="9"/>
+        <v>512</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="7"/>
+        <v>384000</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="8"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="9"/>
+        <v>960</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="9"/>
+        <v>480</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="7"/>
+        <v>384000</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="8"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="9"/>
+        <v>960</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="9"/>
+        <v>1440</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="7"/>
+        <v>480000</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="8"/>
+        <v>333.33333333333331</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>14</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="9"/>
+        <v>2520</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="7"/>
+        <v>420000</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="8"/>
+        <v>166.66666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28:E29" si="10">E27</f>
+        <v>14</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="9"/>
+        <v>2800</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="7"/>
+        <v>420000</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="8"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="9"/>
+        <v>5880</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="7"/>
+        <v>420000</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="8"/>
+        <v>71.428571428571431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555E026-F9FF-4DAF-B7E6-87243EAFBF4E}">
+  <dimension ref="B2:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>MIN(FLOOR((C4+D4)/2,1),5)</f>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2.1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+      <c r="I4">
+        <f>(F4+(H4*G4))</f>
+        <v>2.15</v>
+      </c>
+      <c r="J4">
+        <f>FLOOR(E4*C4*D4*I4,1)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E18" si="0">MIN(FLOOR((C5+D5)/2,1),5)</f>
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f>F4</f>
+        <v>2.1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G18" si="1">G4</f>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>H4</f>
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I18" si="2">(F5+(H5*G5))</f>
+        <v>2.15</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J18" si="3">FLOOR(E5*C5*D5*I5,1)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F18" si="4">F5</f>
+        <v>2.1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H18" si="5">H5</f>
+        <v>0.05</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2.1</v>
       </c>
       <c r="G18">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H18">
-        <f t="shared" si="4"/>
-        <v>506.25</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="6"/>
-        <v>22.5</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="4"/>
-        <v>540</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="6"/>
-        <v>22.5</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>675</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>5</v>
-      </c>
-      <c r="D21">
-        <v>5</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="6"/>
-        <v>22.5</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="4"/>
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="6"/>
-        <v>22.5</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="4"/>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="6"/>
-        <v>22.5</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <v>8</v>
-      </c>
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24">
-        <v>18.5</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="H24">
-        <f t="shared" ref="H24" si="8">(C24*extra)*(D24*extra)*E24*F24*G24</f>
-        <v>3330</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <v>8</v>
-      </c>
-      <c r="D25">
-        <v>10</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="6"/>
-        <v>18.5</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <f>G24</f>
-        <v>0.5</v>
-      </c>
-      <c r="H25">
-        <f t="shared" ref="H25" si="9">(C25*extra)*(D25*extra)*E25*F25*G25</f>
-        <v>3700</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <v>12</v>
-      </c>
-      <c r="D26">
-        <v>14</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="6"/>
-        <v>18.5</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G26">
-        <f>G25</f>
-        <v>0.5</v>
-      </c>
-      <c r="H26">
-        <f>(C26*extra)*(D26*extra)*E26*F26*G26</f>
-        <v>7770</v>
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last change before finding the height of the prefab
</commit_message>
<xml_diff>
--- a/WorkerCalc.xlsx
+++ b/WorkerCalc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Whitefang Greytail\Documents\Visual Studio 2019\Projects\CS2_RealisticPopulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FB9559-C77A-425B-99AF-C9EED3624E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D9CDCC-552F-4E46-B2FE-0C056275CB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Office" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>w</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>buildings</t>
+  </si>
+  <si>
+    <t>w height</t>
+  </si>
+  <si>
+    <t>w/o</t>
+  </si>
+  <si>
+    <t>row</t>
   </si>
 </sst>
 </file>
@@ -427,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3C188A-A917-4627-9F8C-CA03B9A0C4A5}">
-  <dimension ref="C3:N29"/>
+  <dimension ref="C3:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -477,7 +486,7 @@
       </c>
       <c r="H4">
         <f>(C4)*(D4)*E4*F4*G4</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
@@ -489,7 +498,7 @@
       </c>
       <c r="E5">
         <f>E4</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <f>F4</f>
@@ -500,8 +509,8 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H12" si="0">(C5)*(D5)*E5*F5*G5</f>
-        <v>15</v>
+        <f t="shared" ref="H5:H6" si="0">(C5)*(D5)*E5*F5*G5</f>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
@@ -512,20 +521,20 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E12" si="1">E5</f>
-        <v>5</v>
+        <f t="shared" ref="E6:E11" si="1">E5</f>
+        <v>8</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F12" si="2">F5</f>
+        <f t="shared" ref="F6:F11" si="2">F5</f>
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G12" si="3">G5</f>
+        <f t="shared" ref="G6:G8" si="3">G5</f>
         <v>0.5</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
@@ -533,11 +542,11 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
@@ -548,20 +557,20 @@
         <v>0.5</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
+        <f t="shared" ref="H7" si="4">(C7)*(D7)*E7*F7*G7</f>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
@@ -572,8 +581,8 @@
         <v>0.5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <f t="shared" ref="H8:H13" si="5">(C8)*(D8)*E8*F8*G8</f>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
@@ -581,71 +590,71 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f>G8</f>
         <v>0.5</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f t="shared" si="5"/>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
+        <f>G9</f>
         <v>0.5</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>62.5</v>
+        <f t="shared" si="5"/>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
+        <f>G10</f>
         <v>0.5</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f t="shared" si="5"/>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
@@ -653,67 +662,67 @@
         <v>6</v>
       </c>
       <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f>E11</f>
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <f>F11</f>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f>G11</f>
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13">
         <v>6</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="J14">
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <f>E12</f>
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <f>F12</f>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f>G12</f>
+        <v>0.5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15">
         <v>12000</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" t="s">
         <v>11</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M15" t="s">
         <v>10</v>
       </c>
-      <c r="N14">
+      <c r="N15">
         <v>105000</v>
-      </c>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>16</v>
-      </c>
-      <c r="F15">
-        <f>(MIN(FLOOR((C15+D15)/2,1),5))</f>
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>0.5</v>
-      </c>
-      <c r="H15">
-        <f>(C15)*(D15)*E15*F15*G15</f>
-        <v>64</v>
-      </c>
-      <c r="J15">
-        <f>12000*(H15/(C15*D15))</f>
-        <v>192000</v>
-      </c>
-      <c r="K15">
-        <f>12000/(C15*D15)</f>
-        <v>3000</v>
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
@@ -721,63 +730,69 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:E26" si="4">E15</f>
         <v>16</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F29" si="5">(MIN(FLOOR((C16+D16)/2,1),5))</f>
-        <v>3</v>
+        <f>(MIN(FLOOR((C16+D16)/2,1),5))</f>
+        <v>2</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16:G29" si="6">G15</f>
         <v>0.5</v>
       </c>
       <c r="H16">
         <f>(C16)*(D16)*E16*F16*G16</f>
-        <v>192</v>
+        <v>64</v>
+      </c>
+      <c r="I16">
+        <f>(C16)*(D16)*E16*G16*2</f>
+        <v>64</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:J29" si="7">12000*(H16/(C16*D16))</f>
-        <v>288000</v>
+        <f>12000*(H16/(C16*D16))</f>
+        <v>192000</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K29" si="8">12000/(C16*D16)</f>
-        <v>1500</v>
+        <f>12000/(C16*D16)</f>
+        <v>3000</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E17:E27" si="6">E16</f>
         <v>16</v>
       </c>
       <c r="F17">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" ref="F17:F30" si="7">(MIN(FLOOR((C17+D17)/2,1),5))</f>
+        <v>3</v>
       </c>
       <c r="G17">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G17:G30" si="8">G16</f>
         <v>0.5</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:H29" si="9">(C17)*(D17)*E17*F17*G17</f>
-        <v>96</v>
+        <f>(C17)*(D17)*E17*F17*G17</f>
+        <v>192</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I30" si="9">(C17)*(D17)*E17*G17*2</f>
+        <v>128</v>
       </c>
       <c r="J17">
-        <f t="shared" si="7"/>
-        <v>192000</v>
+        <f t="shared" ref="J17:J30" si="10">12000*(H17/(C17*D17))</f>
+        <v>288000</v>
       </c>
       <c r="K17">
-        <f t="shared" si="8"/>
-        <v>2000</v>
+        <f t="shared" ref="K17:K30" si="11">12000/(C17*D17)</f>
+        <v>1500</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
@@ -785,127 +800,143 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="G18">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H30" si="12">(C18)*(D18)*E18*F18*G18</f>
+        <v>96</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="9"/>
+        <v>96</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="10"/>
+        <v>192000</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
         <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="12"/>
+        <v>288</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="9"/>
+        <v>192</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="10"/>
+        <v>288000</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="11"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="9"/>
+        <v>240</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="10"/>
+        <v>384000</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="11"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="12"/>
+        <v>576</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="9"/>
         <v>288</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="7"/>
-        <v>288000</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="8"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="9"/>
-        <v>480</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="7"/>
+      <c r="J21">
+        <f t="shared" si="10"/>
         <v>384000</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="8"/>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="9"/>
-        <v>576</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="7"/>
-        <v>384000</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="8"/>
+      <c r="K21">
+        <f t="shared" si="11"/>
         <v>666.66666666666663</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="9"/>
-        <v>512</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="7"/>
-        <v>384000</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="8"/>
-        <v>750</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
@@ -913,63 +944,71 @@
         <v>4</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="F22">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="G22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H22">
+        <f t="shared" si="12"/>
+        <v>512</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="9"/>
-        <v>960</v>
+        <v>256</v>
       </c>
       <c r="J22">
-        <f t="shared" si="7"/>
-        <v>480000</v>
+        <f t="shared" si="10"/>
+        <v>384000</v>
       </c>
       <c r="K22">
-        <f t="shared" si="8"/>
-        <v>500</v>
+        <f t="shared" si="11"/>
+        <v>750</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="F23">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="G23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H23">
+        <f t="shared" si="12"/>
+        <v>960</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="9"/>
-        <v>480</v>
+        <v>384</v>
       </c>
       <c r="J23">
-        <f t="shared" si="7"/>
-        <v>384000</v>
+        <f t="shared" si="10"/>
+        <v>480000</v>
       </c>
       <c r="K23">
-        <f t="shared" si="8"/>
-        <v>800</v>
+        <f t="shared" si="11"/>
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
@@ -977,63 +1016,71 @@
         <v>5</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="F24">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="G24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H24">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="9"/>
-        <v>1000</v>
+        <v>240</v>
       </c>
       <c r="J24">
-        <f t="shared" si="7"/>
-        <v>480000</v>
+        <f t="shared" si="10"/>
+        <v>384000</v>
       </c>
       <c r="K24">
-        <f t="shared" si="8"/>
-        <v>480</v>
+        <f t="shared" si="11"/>
+        <v>800</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="G25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H25">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="9"/>
-        <v>960</v>
+        <v>400</v>
       </c>
       <c r="J25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>480000</v>
       </c>
       <c r="K25">
-        <f t="shared" si="8"/>
-        <v>500</v>
+        <f t="shared" si="11"/>
+        <v>480</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
@@ -1041,62 +1088,71 @@
         <v>6</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="F26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="G26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H26">
+        <f t="shared" si="12"/>
+        <v>960</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="9"/>
-        <v>1440</v>
+        <v>384</v>
       </c>
       <c r="J26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>480000</v>
       </c>
       <c r="K26">
-        <f t="shared" si="8"/>
-        <v>333.33333333333331</v>
+        <f t="shared" si="11"/>
+        <v>500</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E27">
-        <v>14</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="F27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="G27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H27">
+        <f t="shared" si="12"/>
+        <v>1440</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="9"/>
-        <v>2520</v>
+        <v>576</v>
       </c>
       <c r="J27">
-        <f t="shared" si="7"/>
-        <v>420000</v>
+        <f t="shared" si="10"/>
+        <v>480000</v>
       </c>
       <c r="K27">
-        <f t="shared" si="8"/>
-        <v>166.66666666666666</v>
+        <f t="shared" si="11"/>
+        <v>333.33333333333331</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
@@ -1104,62 +1160,106 @@
         <v>8</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28:E29" si="10">E27</f>
+        <f>E27-2</f>
         <v>14</v>
       </c>
       <c r="F28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="G28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H28">
+        <f t="shared" si="12"/>
+        <v>2520</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="9"/>
-        <v>2800</v>
+        <v>1008</v>
       </c>
       <c r="J28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>420000</v>
       </c>
       <c r="K28">
-        <f t="shared" si="8"/>
-        <v>150</v>
+        <f t="shared" si="11"/>
+        <v>166.66666666666666</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E30" si="13">E28</f>
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="12"/>
+        <v>2800</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="9"/>
+        <v>1120</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="10"/>
+        <v>420000</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="11"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30">
         <v>12</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>14</v>
       </c>
-      <c r="E29">
+      <c r="E30">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="12"/>
+        <v>5880</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="9"/>
+        <v>2352</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="9"/>
-        <v>5880</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="7"/>
         <v>420000</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="8"/>
+      <c r="K30">
+        <f t="shared" si="11"/>
         <v>71.428571428571431</v>
       </c>
     </row>
@@ -1170,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555E026-F9FF-4DAF-B7E6-87243EAFBF4E}">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,7 +1719,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>6</v>
       </c>
@@ -1651,7 +1751,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>6</v>
       </c>
@@ -1681,6 +1781,69 @@
       <c r="J18">
         <f t="shared" si="3"/>
         <v>387</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0.75</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0.25</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22" si="6">(F22+(H22*G22))</f>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22" si="7">FLOOR(E22*C22*D22*I22,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f>F22</f>
+        <v>0.75</v>
+      </c>
+      <c r="G23">
+        <f>G22</f>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0.25</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I24" si="8">(F23+(H23*G23))</f>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:J24" si="9">FLOOR(E23*C23*D23*I23,1)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First change to PDXMods
</commit_message>
<xml_diff>
--- a/WorkerCalc.xlsx
+++ b/WorkerCalc.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Whitefang Greytail\Documents\Visual Studio 2019\Projects\CS2_RealisticPopulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61582F0C-2FA6-40AB-AE8F-32BD45125EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D9CDCC-552F-4E46-B2FE-0C056275CB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{837DFBAA-BE59-4B40-A14A-99C4D03947BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Office" sheetId="1" r:id="rId1"/>
+    <sheet name="Residential" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="extra">Sheet1!$G$1</definedName>
+    <definedName name="extra">Office!$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>w</t>
   </si>
@@ -59,7 +60,31 @@
     <t>workerCell</t>
   </si>
   <si>
-    <t>extra</t>
+    <t>homes</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>lvlMult</t>
+  </si>
+  <si>
+    <t>high density</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>buildings</t>
+  </si>
+  <si>
+    <t>w height</t>
+  </si>
+  <si>
+    <t>w/o</t>
+  </si>
+  <si>
+    <t>row</t>
   </si>
 </sst>
 </file>
@@ -411,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3C188A-A917-4627-9F8C-CA03B9A0C4A5}">
-  <dimension ref="C1:H26"/>
+  <dimension ref="C3:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,15 +448,7 @@
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -451,7 +468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>2</v>
       </c>
@@ -459,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -468,11 +485,11 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f>(C4*extra)*(D4*extra)*E4*F4*G4</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+        <f>(C4)*(D4)*E4*F4*G4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -481,7 +498,7 @@
       </c>
       <c r="E5">
         <f>E4</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <f>F4</f>
@@ -492,11 +509,11 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H12" si="0">(C5*extra)*(D5*extra)*E5*F5*G5</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H5:H6" si="0">(C5)*(D5)*E5*F5*G5</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -504,32 +521,32 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E12" si="1">E5</f>
-        <v>4</v>
+        <f t="shared" ref="E6:E11" si="1">E5</f>
+        <v>8</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F12" si="2">F5</f>
+        <f t="shared" ref="F6:F11" si="2">F5</f>
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G12" si="3">G5</f>
+        <f t="shared" ref="G6:G8" si="3">G5</f>
         <v>0.5</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
@@ -540,20 +557,20 @@
         <v>0.5</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H7" si="4">(C7)*(D7)*E7*F7*G7</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
@@ -564,389 +581,1269 @@
         <v>0.5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H8:H13" si="5">(C8)*(D8)*E8*F8*G8</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f>G8</f>
         <v>0.5</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
+        <f>G9</f>
         <v>0.5</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
+        <f>G10</f>
         <v>0.5</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f>E11</f>
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <f>F11</f>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f>G11</f>
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13">
         <v>6</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>22.5</v>
-      </c>
-      <c r="F15">
-        <f>MIN(FLOOR((C15+D15)/2,1),5)-1</f>
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0.5</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ref="H15:H23" si="4">(C15*extra)*(D15*extra)*E15*F15*G15</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <f>E12</f>
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <f>F12</f>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f>G12</f>
+        <v>0.5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15">
+        <v>12000</v>
+      </c>
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <f>E15</f>
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F26" si="5">(MIN(FLOOR((C16+D16)/2,1),6)-1)</f>
-        <v>1</v>
+        <f>(MIN(FLOOR((C16+D16)/2,1),5))</f>
+        <v>2</v>
       </c>
       <c r="G16">
-        <f>G15</f>
         <v>0.5</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+        <f>(C16)*(D16)*E16*F16*G16</f>
+        <v>64</v>
+      </c>
+      <c r="I16">
+        <f>(C16)*(D16)*E16*G16*2</f>
+        <v>64</v>
+      </c>
+      <c r="J16">
+        <f>12000*(H16/(C16*D16))</f>
+        <v>192000</v>
+      </c>
+      <c r="K16">
+        <f>12000/(C16*D16)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E26" si="6">E16</f>
-        <v>22.5</v>
+        <f t="shared" ref="E17:E27" si="6">E16</f>
+        <v>16</v>
       </c>
       <c r="F17">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" ref="F17:F30" si="7">(MIN(FLOOR((C17+D17)/2,1),5))</f>
+        <v>3</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G24" si="7">G16</f>
+        <f t="shared" ref="G17:G30" si="8">G16</f>
         <v>0.5</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+        <f>(C17)*(D17)*E17*F17*G17</f>
+        <v>192</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I30" si="9">(C17)*(D17)*E17*G17*2</f>
+        <v>128</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J30" si="10">12000*(H17/(C17*D17))</f>
+        <v>288000</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="K17:K30" si="11">12000/(C17*D17)</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="G18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H18">
-        <f t="shared" si="4"/>
-        <v>506.25</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H18:H30" si="12">(C18)*(D18)*E18*F18*G18</f>
+        <v>96</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="9"/>
+        <v>96</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="10"/>
+        <v>192000</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>4</v>
       </c>
       <c r="E19">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="G19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
-        <v>540</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>288</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="9"/>
+        <v>192</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="10"/>
+        <v>288000</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="11"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>5</v>
       </c>
       <c r="E20">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F20">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="G20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H20">
-        <f t="shared" si="4"/>
-        <v>675</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="9"/>
+        <v>240</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="10"/>
+        <v>384000</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="11"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="G21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H21">
-        <f t="shared" si="4"/>
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>576</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="9"/>
+        <v>288</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="10"/>
+        <v>384000</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="11"/>
+        <v>666.66666666666663</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="G22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H22">
-        <f t="shared" si="4"/>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>512</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>256</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="10"/>
+        <v>384000</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="11"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <v>6</v>
       </c>
       <c r="E23">
         <f t="shared" si="6"/>
-        <v>22.5</v>
+        <v>16</v>
       </c>
       <c r="F23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="G23">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="12"/>
+        <v>960</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="9"/>
+        <v>384</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="10"/>
+        <v>480000</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="11"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <v>8</v>
-      </c>
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24">
-        <v>18.5</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H24">
-        <f t="shared" ref="H24" si="8">(C24*extra)*(D24*extra)*E24*F24*G24</f>
-        <v>3330</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="9"/>
+        <v>240</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="10"/>
+        <v>384000</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="11"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E25">
         <f t="shared" si="6"/>
-        <v>18.5</v>
+        <v>16</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="G25">
-        <f>G24</f>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25" si="9">(C25*extra)*(D25*extra)*E25*F25*G25</f>
-        <v>3700</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="9"/>
+        <v>400</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="10"/>
+        <v>480000</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="11"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D26">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <f t="shared" si="6"/>
-        <v>18.5</v>
+        <v>16</v>
       </c>
       <c r="F26">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="12"/>
+        <v>960</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="9"/>
+        <v>384</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="10"/>
+        <v>480000</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="11"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="12"/>
+        <v>1440</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="9"/>
+        <v>576</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="10"/>
+        <v>480000</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="11"/>
+        <v>333.33333333333331</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <f>E27-2</f>
+        <v>14</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="12"/>
+        <v>2520</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="9"/>
+        <v>1008</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="10"/>
+        <v>420000</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="11"/>
+        <v>166.66666666666666</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E30" si="13">E28</f>
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="12"/>
+        <v>2800</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="9"/>
+        <v>1120</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="10"/>
+        <v>420000</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="11"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="12"/>
+        <v>5880</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="9"/>
+        <v>2352</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="10"/>
+        <v>420000</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="11"/>
+        <v>71.428571428571431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555E026-F9FF-4DAF-B7E6-87243EAFBF4E}">
+  <dimension ref="B2:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>MIN(FLOOR((C4+D4)/2,1),5)</f>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2.1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+      <c r="I4">
+        <f>(F4+(H4*G4))</f>
+        <v>2.15</v>
+      </c>
+      <c r="J4">
+        <f>FLOOR(E4*C4*D4*I4,1)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E18" si="0">MIN(FLOOR((C5+D5)/2,1),5)</f>
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f>F4</f>
+        <v>2.1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G18" si="1">G4</f>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>H4</f>
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I18" si="2">(F5+(H5*G5))</f>
+        <v>2.15</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J18" si="3">FLOOR(E5*C5*D5*I5,1)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F18" si="4">F5</f>
+        <v>2.1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H18" si="5">H5</f>
+        <v>0.05</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G26">
-        <f>G25</f>
-        <v>0.5</v>
-      </c>
-      <c r="H26">
-        <f>(C26*extra)*(D26*extra)*E26*F26*G26</f>
-        <v>7770</v>
+        <v>0.05</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>2.15</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0.75</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0.25</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22" si="6">(F22+(H22*G22))</f>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22" si="7">FLOOR(E22*C22*D22*I22,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f>F22</f>
+        <v>0.75</v>
+      </c>
+      <c r="G23">
+        <f>G22</f>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0.25</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I24" si="8">(F23+(H23*G23))</f>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:J24" si="9">FLOOR(E23*C23*D23*I23,1)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>